<commit_message>
RDM-4826 Fixed an error when merging v18 definition.
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v19_RDM-4826_markdown_on_collection_items.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v19_RDM-4826_markdown_on_collection_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59E641C-9F52-5141-A3D1-1B2F1B8BC8F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8FBAB-9DC1-BD48-B0D8-8C8290CE4B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -27557,7 +27557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -29352,7 +29352,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D8" sqref="D8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -29380,7 +29380,7 @@
       <c r="F1" s="176"/>
       <c r="G1" s="176"/>
     </row>
-    <row r="2" spans="1:7" ht="252" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="126" x14ac:dyDescent="0.15">
       <c r="A2" s="174"/>
       <c r="B2" s="174"/>
       <c r="C2" s="175" t="s">
@@ -30011,8 +30011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -30435,6 +30435,9 @@
       <c r="J16" s="84" t="s">
         <v>437</v>
       </c>
+      <c r="K16" s="84" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="85">
@@ -30464,9 +30467,7 @@
       <c r="J17" s="84" t="s">
         <v>439</v>
       </c>
-      <c r="K17" s="84" t="s">
-        <v>469</v>
-      </c>
+      <c r="K17" s="84"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="85">
@@ -30536,6 +30537,9 @@
       <c r="J20" s="84" t="s">
         <v>437</v>
       </c>
+      <c r="K20" s="84" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="85">
@@ -30557,13 +30561,11 @@
         <v>437</v>
       </c>
       <c r="K21" s="84" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="K22" s="84" t="s">
-        <v>471</v>
-      </c>
+      <c r="K22" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RDM-4826 Update latest definition with missing access for AddressUk.
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v19_RDM-4826_markdown_on_collection_items.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v19_RDM-4826_markdown_on_collection_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8FBAB-9DC1-BD48-B0D8-8C8290CE4B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001B41D9-59F3-4C4E-84E1-7E933F3AB999}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3475" uniqueCount="670">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2147,7 +2147,7 @@
     <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2469,6 +2469,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -2693,7 +2700,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="272">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2990,6 +2997,8 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -5454,7 +5463,7 @@
   <dimension ref="A1:AD103"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12616,10 +12625,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12958,20 +12967,20 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="s">
+      <c r="A15" s="220">
+        <v>42737</v>
+      </c>
+      <c r="B15" s="273"/>
+      <c r="C15" s="222" t="s">
         <v>396</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" s="222" t="s">
+        <v>580</v>
+      </c>
+      <c r="E15" s="221" t="s">
         <v>271</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="222" t="s">
         <v>244</v>
       </c>
       <c r="G15" s="7"/>
@@ -12980,7 +12989,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>42736</v>
       </c>
@@ -12989,7 +12998,7 @@
         <v>396</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>270</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
         <v>271</v>
@@ -13012,7 +13021,7 @@
         <v>396</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>474</v>
+        <v>270</v>
       </c>
       <c r="E17" t="s">
         <v>271</v>
@@ -13032,10 +13041,10 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
-        <v>275</v>
+        <v>396</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>276</v>
+        <v>474</v>
       </c>
       <c r="E18" t="s">
         <v>271</v>
@@ -13049,16 +13058,16 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>42736</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="57" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8" t="s">
         <v>275</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E19" t="s">
         <v>271</v>
@@ -13066,17 +13075,22 @@
       <c r="F19" s="8" t="s">
         <v>244</v>
       </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>42736</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="57" t="s">
         <v>275</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E20" t="s">
         <v>271</v>
@@ -13084,11 +13098,6 @@
       <c r="F20" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
     </row>
     <row r="21" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
@@ -13098,8 +13107,8 @@
       <c r="C21" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D21" s="57" t="s">
-        <v>366</v>
+      <c r="D21" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="E21" t="s">
         <v>271</v>
@@ -13107,54 +13116,54 @@
       <c r="F21" s="8" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="92"/>
-      <c r="C22" s="111" t="s">
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+    </row>
+    <row r="22" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D22" s="111" t="s">
+      <c r="D22" s="57" t="s">
+        <v>366</v>
+      </c>
+      <c r="E22" t="s">
+        <v>271</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="92"/>
+      <c r="C23" s="111" t="s">
+        <v>275</v>
+      </c>
+      <c r="D23" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E23" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F22" s="111" t="s">
+      <c r="F23" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="92"/>
-    </row>
-    <row r="23" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="86" t="s">
-        <v>285</v>
-      </c>
-      <c r="D23" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="E23" t="s">
-        <v>271</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-    </row>
-    <row r="24" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="92"/>
+      <c r="K23" s="92"/>
+    </row>
+    <row r="24" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>42736</v>
       </c>
@@ -13163,7 +13172,7 @@
         <v>285</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E24" t="s">
         <v>271</v>
@@ -13177,7 +13186,7 @@
       <c r="J24" s="42"/>
       <c r="K24" s="42"/>
     </row>
-    <row r="25" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>42736</v>
       </c>
@@ -13186,7 +13195,7 @@
         <v>285</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E25" t="s">
         <v>271</v>
@@ -13204,12 +13213,12 @@
       <c r="A26" s="10">
         <v>42736</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="86" t="s">
         <v>285</v>
       </c>
       <c r="D26" s="57" t="s">
-        <v>454</v>
+        <v>311</v>
       </c>
       <c r="E26" t="s">
         <v>271</v>
@@ -13231,8 +13240,8 @@
       <c r="C27" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="D27" s="173" t="s">
-        <v>548</v>
+      <c r="D27" s="57" t="s">
+        <v>454</v>
       </c>
       <c r="E27" t="s">
         <v>271</v>
@@ -13246,51 +13255,51 @@
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
     </row>
-    <row r="28" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B28" s="92"/>
-      <c r="C28" s="123" t="s">
+    <row r="28" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="D28" s="111" t="s">
-        <v>474</v>
-      </c>
-      <c r="E28" s="93" t="s">
+      <c r="D28" s="173" t="s">
+        <v>548</v>
+      </c>
+      <c r="E28" t="s">
         <v>271</v>
       </c>
-      <c r="F28" s="111" t="s">
+      <c r="F28" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G28" s="92"/>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-    </row>
-    <row r="29" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="7"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+    </row>
+    <row r="29" spans="1:11" s="93" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="92"/>
       <c r="C29" s="123" t="s">
         <v>285</v>
       </c>
-      <c r="D29" s="59" t="s">
-        <v>489</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" s="111" t="s">
+        <v>474</v>
+      </c>
+      <c r="E29" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="92"/>
+      <c r="K29" s="92"/>
     </row>
     <row r="30" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
@@ -13300,8 +13309,8 @@
       <c r="C30" s="123" t="s">
         <v>285</v>
       </c>
-      <c r="D30" s="57" t="s">
-        <v>478</v>
+      <c r="D30" s="59" t="s">
+        <v>489</v>
       </c>
       <c r="E30" t="s">
         <v>271</v>
@@ -13315,16 +13324,16 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
         <v>42736</v>
       </c>
       <c r="B31" s="7"/>
-      <c r="C31" s="57" t="s">
-        <v>329</v>
+      <c r="C31" s="123" t="s">
+        <v>285</v>
       </c>
       <c r="D31" s="57" t="s">
-        <v>332</v>
+        <v>478</v>
       </c>
       <c r="E31" t="s">
         <v>271</v>
@@ -13332,7 +13341,7 @@
       <c r="F31" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G31" s="8"/>
+      <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -13342,12 +13351,12 @@
       <c r="A32" s="10">
         <v>42736</v>
       </c>
-      <c r="B32" s="10"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="57" t="s">
         <v>329</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E32" t="s">
         <v>271</v>
@@ -13370,7 +13379,7 @@
         <v>329</v>
       </c>
       <c r="D33" s="57" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E33" t="s">
         <v>271</v>
@@ -13393,7 +13402,7 @@
         <v>329</v>
       </c>
       <c r="D34" s="57" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E34" t="s">
         <v>271</v>
@@ -13416,7 +13425,7 @@
         <v>329</v>
       </c>
       <c r="D35" s="57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E35" t="s">
         <v>271</v>
@@ -13439,7 +13448,7 @@
         <v>329</v>
       </c>
       <c r="D36" s="57" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E36" t="s">
         <v>271</v>
@@ -13462,7 +13471,7 @@
         <v>329</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E37" t="s">
         <v>271</v>
@@ -13485,7 +13494,7 @@
         <v>329</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="E38" t="s">
         <v>271</v>
@@ -13508,7 +13517,7 @@
         <v>329</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>348</v>
+        <v>364</v>
       </c>
       <c r="E39" t="s">
         <v>271</v>
@@ -13531,7 +13540,7 @@
         <v>329</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E40" t="s">
         <v>271</v>
@@ -13545,51 +13554,51 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B41" s="110"/>
-      <c r="C41" s="112" t="s">
+    <row r="41" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="57" t="s">
         <v>329</v>
       </c>
-      <c r="D41" s="111" t="s">
+      <c r="D41" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="E41" t="s">
+        <v>271</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B42" s="110"/>
+      <c r="C42" s="112" t="s">
+        <v>329</v>
+      </c>
+      <c r="D42" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E41" s="93" t="s">
+      <c r="E42" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F41" s="111" t="s">
+      <c r="F42" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G41" s="111"/>
-      <c r="H41" s="115"/>
-      <c r="I41" s="115"/>
-      <c r="J41" s="115"/>
-      <c r="K41" s="115"/>
-    </row>
-    <row r="42" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="57" t="s">
-        <v>373</v>
-      </c>
-      <c r="D42" s="57" t="s">
-        <v>332</v>
-      </c>
-      <c r="E42" t="s">
-        <v>271</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
+      <c r="G42" s="111"/>
+      <c r="H42" s="115"/>
+      <c r="I42" s="115"/>
+      <c r="J42" s="115"/>
+      <c r="K42" s="115"/>
     </row>
     <row r="43" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="10">
@@ -13600,7 +13609,7 @@
         <v>373</v>
       </c>
       <c r="D43" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E43" t="s">
         <v>271</v>
@@ -13623,7 +13632,7 @@
         <v>373</v>
       </c>
       <c r="D44" s="57" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E44" t="s">
         <v>271</v>
@@ -13646,7 +13655,7 @@
         <v>373</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>387</v>
+        <v>336</v>
       </c>
       <c r="E45" t="s">
         <v>271</v>
@@ -13660,97 +13669,97 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B46" s="110"/>
-      <c r="C46" s="112" t="s">
+    <row r="46" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="D46" s="111" t="s">
+      <c r="D46" s="57" t="s">
+        <v>387</v>
+      </c>
+      <c r="E46" t="s">
+        <v>271</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B47" s="110"/>
+      <c r="C47" s="112" t="s">
+        <v>373</v>
+      </c>
+      <c r="D47" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E46" s="93" t="s">
+      <c r="E47" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F46" s="111" t="s">
+      <c r="F47" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G46" s="111"/>
-      <c r="H46" s="115"/>
-      <c r="I46" s="115"/>
-      <c r="J46" s="115"/>
-      <c r="K46" s="115"/>
-    </row>
-    <row r="47" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="8" t="s">
+      <c r="G47" s="111"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="115"/>
+      <c r="J47" s="115"/>
+      <c r="K47" s="115"/>
+    </row>
+    <row r="48" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>271</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F48" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-    </row>
-    <row r="48" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="110">
-        <v>42736</v>
-      </c>
-      <c r="B48" s="110"/>
-      <c r="C48" s="111" t="s">
+      <c r="G48" s="8"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" s="93" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="110">
+        <v>42736</v>
+      </c>
+      <c r="B49" s="110"/>
+      <c r="C49" s="111" t="s">
         <v>392</v>
       </c>
-      <c r="D48" s="111" t="s">
+      <c r="D49" s="111" t="s">
         <v>474</v>
       </c>
-      <c r="E48" s="93" t="s">
+      <c r="E49" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="F48" s="111" t="s">
+      <c r="F49" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="G48" s="111"/>
-      <c r="H48" s="115"/>
-      <c r="I48" s="115"/>
-      <c r="J48" s="115"/>
-      <c r="K48" s="115"/>
-    </row>
-    <row r="49" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" t="s">
-        <v>271</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
+      <c r="G49" s="111"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="115"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="115"/>
     </row>
     <row r="50" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="10">
@@ -13760,8 +13769,8 @@
       <c r="C50" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D50" s="225" t="s">
-        <v>603</v>
+      <c r="D50" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="E50" t="s">
         <v>271</v>
@@ -13783,8 +13792,8 @@
       <c r="C51" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D51" s="242" t="s">
-        <v>333</v>
+      <c r="D51" s="225" t="s">
+        <v>603</v>
       </c>
       <c r="E51" t="s">
         <v>271</v>
@@ -13807,7 +13816,7 @@
         <v>397</v>
       </c>
       <c r="D52" s="242" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E52" t="s">
         <v>271</v>
@@ -13821,30 +13830,30 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" s="146" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="197">
-        <v>42736</v>
-      </c>
-      <c r="B53" s="197"/>
-      <c r="C53" s="198" t="s">
+    <row r="53" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D53" s="198" t="s">
-        <v>580</v>
-      </c>
-      <c r="E53" s="199" t="s">
+      <c r="D53" s="242" t="s">
+        <v>336</v>
+      </c>
+      <c r="E53" t="s">
         <v>271</v>
       </c>
-      <c r="F53" s="198" t="s">
+      <c r="F53" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="G53" s="147"/>
-      <c r="H53" s="148"/>
-      <c r="I53" s="148"/>
-      <c r="J53" s="148"/>
-      <c r="K53" s="148"/>
-    </row>
-    <row r="54" spans="1:11" s="146" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G53" s="8"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:11" s="146" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="197">
         <v>42736</v>
       </c>
@@ -13853,7 +13862,7 @@
         <v>397</v>
       </c>
       <c r="D54" s="198" t="s">
-        <v>75</v>
+        <v>580</v>
       </c>
       <c r="E54" s="199" t="s">
         <v>271</v>
@@ -13861,6 +13870,11 @@
       <c r="F54" s="198" t="s">
         <v>244</v>
       </c>
+      <c r="G54" s="147"/>
+      <c r="H54" s="148"/>
+      <c r="I54" s="148"/>
+      <c r="J54" s="148"/>
+      <c r="K54" s="148"/>
     </row>
     <row r="55" spans="1:11" s="146" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="197">
@@ -13871,7 +13885,7 @@
         <v>397</v>
       </c>
       <c r="D55" s="198" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E55" s="199" t="s">
         <v>271</v>
@@ -13889,7 +13903,7 @@
         <v>397</v>
       </c>
       <c r="D56" s="198" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E56" s="199" t="s">
         <v>271</v>
@@ -13898,7 +13912,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="167" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" s="146" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="197">
         <v>42736</v>
       </c>
@@ -13907,7 +13921,7 @@
         <v>397</v>
       </c>
       <c r="D57" s="198" t="s">
-        <v>270</v>
+        <v>83</v>
       </c>
       <c r="E57" s="199" t="s">
         <v>271</v>
@@ -13915,11 +13929,6 @@
       <c r="F57" s="198" t="s">
         <v>244</v>
       </c>
-      <c r="G57" s="169"/>
-      <c r="H57" s="170"/>
-      <c r="I57" s="170"/>
-      <c r="J57" s="170"/>
-      <c r="K57" s="170"/>
     </row>
     <row r="58" spans="1:11" s="167" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="197">
@@ -13930,7 +13939,7 @@
         <v>397</v>
       </c>
       <c r="D58" s="198" t="s">
-        <v>88</v>
+        <v>270</v>
       </c>
       <c r="E58" s="199" t="s">
         <v>271</v>
@@ -13944,39 +13953,44 @@
       <c r="J58" s="170"/>
       <c r="K58" s="170"/>
     </row>
-    <row r="59" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="200">
-        <v>42736</v>
-      </c>
-      <c r="B59" s="200"/>
-      <c r="C59" s="201" t="s">
+    <row r="59" spans="1:11" s="167" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="197">
+        <v>42736</v>
+      </c>
+      <c r="B59" s="197"/>
+      <c r="C59" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D59" s="201" t="s">
+      <c r="D59" s="198" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" s="199" t="s">
+        <v>271</v>
+      </c>
+      <c r="F59" s="198" t="s">
+        <v>244</v>
+      </c>
+      <c r="G59" s="169"/>
+      <c r="H59" s="170"/>
+      <c r="I59" s="170"/>
+      <c r="J59" s="170"/>
+      <c r="K59" s="170"/>
+    </row>
+    <row r="60" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="200">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="200"/>
+      <c r="C60" s="201" t="s">
+        <v>397</v>
+      </c>
+      <c r="D60" s="201" t="s">
         <v>474</v>
       </c>
-      <c r="E59" s="202" t="s">
+      <c r="E60" s="202" t="s">
         <v>271</v>
       </c>
-      <c r="F59" s="201" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="197">
-        <v>42736</v>
-      </c>
-      <c r="B60" s="197"/>
-      <c r="C60" s="198" t="s">
-        <v>397</v>
-      </c>
-      <c r="D60" s="203" t="s">
-        <v>494</v>
-      </c>
-      <c r="E60" s="199" t="s">
-        <v>271</v>
-      </c>
-      <c r="F60" s="198" t="s">
+      <c r="F60" s="201" t="s">
         <v>244</v>
       </c>
     </row>
@@ -13988,8 +14002,8 @@
       <c r="C61" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D61" s="204" t="s">
-        <v>79</v>
+      <c r="D61" s="203" t="s">
+        <v>494</v>
       </c>
       <c r="E61" s="199" t="s">
         <v>271</v>
@@ -14007,7 +14021,7 @@
         <v>397</v>
       </c>
       <c r="D62" s="204" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E62" s="199" t="s">
         <v>271</v>
@@ -14025,7 +14039,7 @@
         <v>397</v>
       </c>
       <c r="D63" s="204" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E63" s="199" t="s">
         <v>271</v>
@@ -14042,8 +14056,8 @@
       <c r="C64" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D64" s="203" t="s">
-        <v>581</v>
+      <c r="D64" s="204" t="s">
+        <v>68</v>
       </c>
       <c r="E64" s="199" t="s">
         <v>271</v>
@@ -14061,7 +14075,7 @@
         <v>397</v>
       </c>
       <c r="D65" s="203" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E65" s="199" t="s">
         <v>271</v>
@@ -14079,7 +14093,7 @@
         <v>397</v>
       </c>
       <c r="D66" s="203" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E66" s="199" t="s">
         <v>271</v>
@@ -14097,7 +14111,7 @@
         <v>397</v>
       </c>
       <c r="D67" s="203" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E67" s="199" t="s">
         <v>271</v>
@@ -14115,7 +14129,7 @@
         <v>397</v>
       </c>
       <c r="D68" s="203" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E68" s="199" t="s">
         <v>271</v>
@@ -14133,7 +14147,7 @@
         <v>397</v>
       </c>
       <c r="D69" s="203" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E69" s="199" t="s">
         <v>271</v>
@@ -14151,7 +14165,7 @@
         <v>397</v>
       </c>
       <c r="D70" s="203" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E70" s="199" t="s">
         <v>271</v>
@@ -14169,7 +14183,7 @@
         <v>397</v>
       </c>
       <c r="D71" s="203" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E71" s="199" t="s">
         <v>271</v>
@@ -14187,7 +14201,7 @@
         <v>397</v>
       </c>
       <c r="D72" s="203" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E72" s="199" t="s">
         <v>271</v>
@@ -14205,7 +14219,7 @@
         <v>397</v>
       </c>
       <c r="D73" s="203" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E73" s="199" t="s">
         <v>271</v>
@@ -14215,20 +14229,20 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="205">
-        <v>42736</v>
-      </c>
-      <c r="B74" s="205"/>
-      <c r="C74" s="206" t="s">
+      <c r="A74" s="197">
+        <v>42736</v>
+      </c>
+      <c r="B74" s="197"/>
+      <c r="C74" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D74" s="207" t="s">
-        <v>591</v>
-      </c>
-      <c r="E74" s="208" t="s">
+      <c r="D74" s="203" t="s">
+        <v>590</v>
+      </c>
+      <c r="E74" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="F74" s="206" t="s">
+      <c r="F74" s="198" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14241,7 +14255,7 @@
         <v>397</v>
       </c>
       <c r="D75" s="207" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E75" s="208" t="s">
         <v>271</v>
@@ -14251,20 +14265,20 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="197">
-        <v>42736</v>
-      </c>
-      <c r="B76" s="197"/>
-      <c r="C76" s="198" t="s">
+      <c r="A76" s="205">
+        <v>42736</v>
+      </c>
+      <c r="B76" s="205"/>
+      <c r="C76" s="206" t="s">
         <v>397</v>
       </c>
-      <c r="D76" s="203" t="s">
-        <v>520</v>
-      </c>
-      <c r="E76" s="199" t="s">
+      <c r="D76" s="207" t="s">
+        <v>592</v>
+      </c>
+      <c r="E76" s="208" t="s">
         <v>271</v>
       </c>
-      <c r="F76" s="198" t="s">
+      <c r="F76" s="206" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14277,7 +14291,7 @@
         <v>397</v>
       </c>
       <c r="D77" s="203" t="s">
-        <v>478</v>
+        <v>520</v>
       </c>
       <c r="E77" s="199" t="s">
         <v>271</v>
@@ -14287,20 +14301,20 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="209">
-        <v>42736</v>
-      </c>
-      <c r="B78" s="209"/>
-      <c r="C78" s="210" t="s">
+      <c r="A78" s="197">
+        <v>42736</v>
+      </c>
+      <c r="B78" s="197"/>
+      <c r="C78" s="198" t="s">
         <v>397</v>
       </c>
-      <c r="D78" s="210" t="s">
-        <v>334</v>
-      </c>
-      <c r="E78" s="211" t="s">
+      <c r="D78" s="203" t="s">
+        <v>478</v>
+      </c>
+      <c r="E78" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="F78" s="210" t="s">
+      <c r="F78" s="198" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14313,7 +14327,7 @@
         <v>397</v>
       </c>
       <c r="D79" s="210" t="s">
-        <v>593</v>
+        <v>334</v>
       </c>
       <c r="E79" s="211" t="s">
         <v>271</v>
@@ -14331,7 +14345,7 @@
         <v>397</v>
       </c>
       <c r="D80" s="210" t="s">
-        <v>337</v>
+        <v>593</v>
       </c>
       <c r="E80" s="211" t="s">
         <v>271</v>
@@ -14349,7 +14363,7 @@
         <v>397</v>
       </c>
       <c r="D81" s="210" t="s">
-        <v>594</v>
+        <v>337</v>
       </c>
       <c r="E81" s="211" t="s">
         <v>271</v>
@@ -14366,8 +14380,8 @@
       <c r="C82" s="210" t="s">
         <v>397</v>
       </c>
-      <c r="D82" s="212" t="s">
-        <v>338</v>
+      <c r="D82" s="210" t="s">
+        <v>594</v>
       </c>
       <c r="E82" s="211" t="s">
         <v>271</v>
@@ -14385,7 +14399,7 @@
         <v>397</v>
       </c>
       <c r="D83" s="212" t="s">
-        <v>595</v>
+        <v>338</v>
       </c>
       <c r="E83" s="211" t="s">
         <v>271</v>
@@ -14403,7 +14417,7 @@
         <v>397</v>
       </c>
       <c r="D84" s="212" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E84" s="211" t="s">
         <v>271</v>
@@ -14421,7 +14435,7 @@
         <v>397</v>
       </c>
       <c r="D85" s="212" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E85" s="211" t="s">
         <v>271</v>
@@ -14439,7 +14453,7 @@
         <v>397</v>
       </c>
       <c r="D86" s="212" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E86" s="211" t="s">
         <v>271</v>
@@ -14449,20 +14463,20 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="241">
-        <v>42736</v>
-      </c>
-      <c r="B87" s="241"/>
-      <c r="C87" s="258" t="s">
-        <v>602</v>
-      </c>
-      <c r="D87" s="242" t="s">
-        <v>296</v>
-      </c>
-      <c r="E87" s="245" t="s">
+      <c r="A87" s="209">
+        <v>42736</v>
+      </c>
+      <c r="B87" s="209"/>
+      <c r="C87" s="210" t="s">
+        <v>397</v>
+      </c>
+      <c r="D87" s="212" t="s">
+        <v>598</v>
+      </c>
+      <c r="E87" s="211" t="s">
         <v>271</v>
       </c>
-      <c r="F87" s="225" t="s">
+      <c r="F87" s="210" t="s">
         <v>244</v>
       </c>
     </row>
@@ -14475,7 +14489,7 @@
         <v>602</v>
       </c>
       <c r="D88" s="242" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="E88" s="245" t="s">
         <v>271</v>
@@ -14493,7 +14507,7 @@
         <v>602</v>
       </c>
       <c r="D89" s="242" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E89" s="245" t="s">
         <v>271</v>
@@ -14506,12 +14520,12 @@
       <c r="A90" s="241">
         <v>42736</v>
       </c>
-      <c r="B90" s="245"/>
+      <c r="B90" s="241"/>
       <c r="C90" s="258" t="s">
         <v>602</v>
       </c>
       <c r="D90" s="242" t="s">
-        <v>454</v>
+        <v>311</v>
       </c>
       <c r="E90" s="245" t="s">
         <v>271</v>
@@ -14524,12 +14538,12 @@
       <c r="A91" s="241">
         <v>42736</v>
       </c>
-      <c r="B91" s="246"/>
+      <c r="B91" s="245"/>
       <c r="C91" s="258" t="s">
         <v>602</v>
       </c>
-      <c r="D91" s="258" t="s">
-        <v>474</v>
+      <c r="D91" s="242" t="s">
+        <v>454</v>
       </c>
       <c r="E91" s="245" t="s">
         <v>271</v>
@@ -14542,12 +14556,12 @@
       <c r="A92" s="241">
         <v>42736</v>
       </c>
-      <c r="B92" s="245"/>
+      <c r="B92" s="246"/>
       <c r="C92" s="258" t="s">
         <v>602</v>
       </c>
       <c r="D92" s="258" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="E92" s="245" t="s">
         <v>271</v>
@@ -14565,12 +14579,30 @@
         <v>602</v>
       </c>
       <c r="D93" s="258" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="E93" s="245" t="s">
         <v>271</v>
       </c>
       <c r="F93" s="225" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="241">
+        <v>42736</v>
+      </c>
+      <c r="B94" s="245"/>
+      <c r="C94" s="258" t="s">
+        <v>602</v>
+      </c>
+      <c r="D94" s="258" t="s">
+        <v>478</v>
+      </c>
+      <c r="E94" s="245" t="s">
+        <v>271</v>
+      </c>
+      <c r="F94" s="225" t="s">
         <v>244</v>
       </c>
     </row>
@@ -15970,8 +16002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV95"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27557,7 +27589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -29351,8 +29383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -30011,7 +30043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -30578,7 +30610,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30649,7 +30681,9 @@
       <c r="E3" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="272" t="s">
+        <v>164</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -30669,7 +30703,9 @@
       <c r="E4" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="240">
+        <v>2</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -30689,7 +30725,9 @@
       <c r="E5" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="240">
+        <v>1</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -30709,7 +30747,9 @@
       <c r="E6" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="240">
+        <v>4</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -30729,7 +30769,9 @@
       <c r="E7" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="240">
+        <v>3</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -30749,7 +30791,9 @@
       <c r="E8" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="240">
+        <v>5</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -30769,7 +30813,9 @@
       <c r="E9" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="240">
+        <v>2</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -30789,7 +30835,7 @@
       <c r="E10" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="240"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -30849,7 +30895,9 @@
       <c r="E13" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="240">
+        <v>4</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>

</xml_diff>